<commit_message>
updates to subtractions FLP data clarity
</commit_message>
<xml_diff>
--- a/Data/NES_FLP_Microscopy.xlsx
+++ b/Data/NES_FLP_Microscopy.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://outlookuga-my.sharepoint.com/personal/ccz99536_uga_edu/Documents/Cruises/NES_CCS_Comparison/AcidotropicManuscript/AcidotropicDyes/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{08F08B38-3099-BE48-ADAA-42526245C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0C54E781-2EA2-FF41-8D0E-E1FC232F858E}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{08F08B38-3099-BE48-ADAA-42526245C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3548C59-C3F3-FF4A-B729-AD179945E9F4}"/>
   <bookViews>
     <workbookView xWindow="1980" yWindow="2780" windowWidth="26440" windowHeight="15440" xr2:uid="{29EB5122-8F0E-0A4E-B3B4-C4828C094E0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
   <si>
     <t>Station</t>
   </si>
@@ -160,6 +160,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -482,7 +486,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -636,32 +640,32 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2">
-        <v>310</v>
+        <v>57</v>
       </c>
       <c r="F4" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G4" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H4" s="2">
-        <f t="shared" ref="H4:H31" si="0">F4/(F4+E4)*100</f>
-        <v>1.89873417721519</v>
+        <f t="shared" ref="H4:H27" si="0">F4/(F4+E4)*100</f>
+        <v>3.3898305084745761</v>
       </c>
       <c r="I4" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
@@ -683,35 +687,35 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E5" s="2">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="G5" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="H5" s="2">
         <f t="shared" si="0"/>
-        <v>29.787234042553191</v>
+        <v>5.2631578947368416</v>
       </c>
       <c r="I5" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J5" s="2">
-        <v>27.88823404</v>
+        <v>1.870169492</v>
       </c>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -741,20 +745,20 @@
         <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E6" s="2">
-        <v>57</v>
+        <v>26</v>
       </c>
       <c r="F6" s="2">
         <v>2</v>
       </c>
       <c r="G6" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="H6" s="2">
         <f t="shared" si="0"/>
-        <v>3.3898305084745761</v>
+        <v>7.1428571428571423</v>
       </c>
       <c r="I6" s="2">
         <v>3</v>
@@ -788,26 +792,26 @@
         <v>12</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E7" s="2">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="0"/>
-        <v>5.2631578947368416</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="I7" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" s="2">
-        <v>1.870169492</v>
+        <v>4.6218487389999998</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -834,26 +838,26 @@
         <v>7</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E8" s="2">
-        <v>26</v>
+        <v>50</v>
       </c>
       <c r="F8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G8" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="2">
         <f t="shared" si="0"/>
-        <v>7.1428571428571423</v>
+        <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
@@ -881,29 +885,29 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E9" s="2">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="F9" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="0"/>
-        <v>11.76470588235294</v>
+        <v>10</v>
       </c>
       <c r="I9" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2">
-        <v>4.6218487389999998</v>
+        <v>10</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -924,32 +928,32 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E10" s="2">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F10" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="G10" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8.5714285714285712</v>
       </c>
       <c r="I10" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
@@ -971,35 +975,35 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E11" s="2">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="F11" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G11" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9.5238095238095237</v>
       </c>
       <c r="I11" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J11" s="2">
-        <v>10</v>
+        <v>0.95238095239999998</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1026,26 +1030,26 @@
         <v>7</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E12" s="2">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F12" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G12" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H12" s="2">
         <f t="shared" si="0"/>
-        <v>8.5714285714285712</v>
+        <v>0</v>
       </c>
       <c r="I12" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
@@ -1073,29 +1077,29 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E13" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F13" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G13" s="2">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="0"/>
-        <v>9.5238095238095237</v>
+        <v>18.181818181818183</v>
       </c>
       <c r="I13" s="2">
         <v>3</v>
       </c>
       <c r="J13" s="2">
-        <v>0.95238095239999998</v>
+        <v>18.18181818</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1122,26 +1126,26 @@
         <v>7</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E14" s="2">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="F14" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G14" s="2">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="I14" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
@@ -1169,29 +1173,29 @@
         <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E15" s="2">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="F15" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G15" s="2">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="0"/>
-        <v>18.181818181818183</v>
+        <v>27.27272727272727</v>
       </c>
       <c r="I15" s="2">
         <v>3</v>
       </c>
       <c r="J15" s="2">
-        <v>18.18181818</v>
+        <v>2.2727272730000001</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1212,32 +1216,32 @@
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E16" s="2">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F16" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="2">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>3.4482758620689653</v>
       </c>
       <c r="I16" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
@@ -1259,35 +1263,35 @@
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E17" s="2">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="F17" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" si="0"/>
-        <v>27.27272727272727</v>
+        <v>12.5</v>
       </c>
       <c r="I17" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J17" s="2">
-        <v>2.2727272730000001</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1314,13 +1318,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E18" s="2">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="F18" s="2">
         <v>1</v>
@@ -1330,10 +1334,10 @@
       </c>
       <c r="H18" s="2">
         <f t="shared" si="0"/>
-        <v>3.4482758620689653</v>
+        <v>4.7619047619047619</v>
       </c>
       <c r="I18" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
@@ -1361,29 +1365,29 @@
         <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E19" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F19" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="2">
         <v>3</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="0"/>
-        <v>12.5</v>
+        <v>7.6923076923076925</v>
       </c>
       <c r="I19" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J19" s="2">
-        <v>9.0500000000000007</v>
+        <v>2.9304029300000001</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1413,20 +1417,20 @@
         <v>12</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E20" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F20" s="2">
         <v>1</v>
       </c>
       <c r="G20" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="0"/>
-        <v>4.7619047619047619</v>
+        <v>4.5454545454545459</v>
       </c>
       <c r="I20" s="2">
         <v>3</v>
@@ -1460,26 +1464,26 @@
         <v>12</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E21" s="2">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="F21" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G21" s="2">
-        <v>3</v>
+        <v>11</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="0"/>
-        <v>7.6923076923076925</v>
+        <v>12.195121951219512</v>
       </c>
       <c r="I21" s="2">
         <v>3</v>
       </c>
       <c r="J21" s="2">
-        <v>2.9304029300000001</v>
+        <v>7.6496674059999998</v>
       </c>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1500,7 +1504,7 @@
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>7</v>
@@ -1509,23 +1513,23 @@
         <v>12</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E22" s="2">
-        <v>21</v>
+        <v>79</v>
       </c>
       <c r="F22" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G22" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="0"/>
-        <v>4.5454545454545459</v>
+        <v>2.4691358024691357</v>
       </c>
       <c r="I22" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
@@ -1547,7 +1551,7 @@
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>10</v>
@@ -1556,26 +1560,26 @@
         <v>12</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E23" s="2">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F23" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G23" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H23" s="2">
         <f t="shared" si="0"/>
-        <v>12.195121951219512</v>
+        <v>20</v>
       </c>
       <c r="I23" s="2">
         <v>3</v>
       </c>
       <c r="J23" s="2">
-        <v>7.6496674059999998</v>
+        <v>17.53</v>
       </c>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1602,26 +1606,26 @@
         <v>7</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E24" s="2">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="F24" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="0"/>
-        <v>2.4691358024691357</v>
+        <v>1.4084507042253522</v>
       </c>
       <c r="I24" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
@@ -1649,29 +1653,29 @@
         <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E25" s="2">
-        <v>8</v>
+        <v>100</v>
       </c>
       <c r="F25" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="G25" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H25" s="2">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="I25" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J25" s="2">
-        <v>17.53</v>
+        <v>-1.4084507040000001</v>
       </c>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -1691,30 +1695,30 @@
       <c r="Z25" s="2"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <v>9</v>
+      <c r="A26" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E26" s="2">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="F26" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="G26" s="2">
-        <v>2</v>
+        <v>60</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="0"/>
-        <v>1.4084507042253522</v>
+        <v>26.388888888888889</v>
       </c>
       <c r="I26" s="2">
         <v>3</v>
@@ -1738,36 +1742,36 @@
       <c r="Z26" s="2"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <v>9</v>
+      <c r="A27" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E27" s="2">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="F27" s="2">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H27" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>27.083333333333332</v>
       </c>
       <c r="I27" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J27" s="2">
-        <v>-1.4084507040000001</v>
+        <v>0.69444444439999997</v>
       </c>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -1787,34 +1791,15 @@
       <c r="Z27" s="2"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E28" s="2">
-        <v>27</v>
-      </c>
-      <c r="F28" s="2">
-        <v>2</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2</v>
-      </c>
-      <c r="H28" s="2">
-        <f t="shared" si="0"/>
-        <v>6.8965517241379306</v>
-      </c>
-      <c r="I28" s="2">
-        <v>1</v>
-      </c>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -1834,37 +1819,16 @@
       <c r="Z28" s="2"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E29" s="2">
-        <v>5</v>
-      </c>
-      <c r="F29" s="2">
-        <v>5</v>
-      </c>
-      <c r="G29" s="2">
-        <v>7</v>
-      </c>
-      <c r="H29" s="2">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="I29" s="2">
-        <v>3</v>
-      </c>
-      <c r="J29" s="2">
-        <v>43.103448280000002</v>
-      </c>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
+      <c r="H29" s="2"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
       <c r="M29" s="2"/>
@@ -1883,34 +1847,15 @@
       <c r="Z29" s="2"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E30" s="2">
-        <v>53</v>
-      </c>
-      <c r="F30" s="2">
-        <v>19</v>
-      </c>
-      <c r="G30" s="2">
-        <v>60</v>
-      </c>
-      <c r="H30" s="2">
-        <f t="shared" si="0"/>
-        <v>26.388888888888889</v>
-      </c>
-      <c r="I30" s="2">
-        <v>3</v>
-      </c>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -1930,37 +1875,16 @@
       <c r="Z30" s="2"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E31" s="2">
-        <v>35</v>
-      </c>
-      <c r="F31" s="2">
-        <v>13</v>
-      </c>
-      <c r="G31" s="2">
-        <v>15</v>
-      </c>
-      <c r="H31" s="2">
-        <f t="shared" si="0"/>
-        <v>27.083333333333332</v>
-      </c>
-      <c r="I31" s="2">
-        <v>3</v>
-      </c>
-      <c r="J31" s="2">
-        <v>0.69444444439999997</v>
-      </c>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
       <c r="M31" s="2"/>
@@ -28999,16 +28923,6 @@
       <c r="Z996" s="2"/>
     </row>
     <row r="997" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A997" s="2"/>
-      <c r="B997" s="2"/>
-      <c r="C997" s="2"/>
-      <c r="D997" s="2"/>
-      <c r="E997" s="2"/>
-      <c r="F997" s="2"/>
-      <c r="G997" s="2"/>
-      <c r="H997" s="2"/>
-      <c r="I997" s="2"/>
-      <c r="J997" s="2"/>
       <c r="K997" s="2"/>
       <c r="L997" s="2"/>
       <c r="M997" s="2"/>
@@ -29027,16 +28941,6 @@
       <c r="Z997" s="2"/>
     </row>
     <row r="998" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A998" s="2"/>
-      <c r="B998" s="2"/>
-      <c r="C998" s="2"/>
-      <c r="D998" s="2"/>
-      <c r="E998" s="2"/>
-      <c r="F998" s="2"/>
-      <c r="G998" s="2"/>
-      <c r="H998" s="2"/>
-      <c r="I998" s="2"/>
-      <c r="J998" s="2"/>
       <c r="K998" s="2"/>
       <c r="L998" s="2"/>
       <c r="M998" s="2"/>
@@ -29055,16 +28959,6 @@
       <c r="Z998" s="2"/>
     </row>
     <row r="999" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A999" s="2"/>
-      <c r="B999" s="2"/>
-      <c r="C999" s="2"/>
-      <c r="D999" s="2"/>
-      <c r="E999" s="2"/>
-      <c r="F999" s="2"/>
-      <c r="G999" s="2"/>
-      <c r="H999" s="2"/>
-      <c r="I999" s="2"/>
-      <c r="J999" s="2"/>
       <c r="K999" s="2"/>
       <c r="L999" s="2"/>
       <c r="M999" s="2"/>
@@ -29083,16 +28977,6 @@
       <c r="Z999" s="2"/>
     </row>
     <row r="1000" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1000" s="2"/>
-      <c r="B1000" s="2"/>
-      <c r="C1000" s="2"/>
-      <c r="D1000" s="2"/>
-      <c r="E1000" s="2"/>
-      <c r="F1000" s="2"/>
-      <c r="G1000" s="2"/>
-      <c r="H1000" s="2"/>
-      <c r="I1000" s="2"/>
-      <c r="J1000" s="2"/>
       <c r="K1000" s="2"/>
       <c r="L1000" s="2"/>
       <c r="M1000" s="2"/>

</xml_diff>